<commit_message>
2021-4-6 slam learn update
</commit_message>
<xml_diff>
--- a/Robotics_and_Slam/2_slam_paper.xlsx
+++ b/Robotics_and_Slam/2_slam_paper.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>title</t>
   </si>
@@ -67,7 +67,7 @@
 辅助vSLAM的研究成果稍逊一筹.目前语义vSLAM的相关研究尚不完善,但是最具潜力研究方向之一</t>
   </si>
   <si>
-    <t>A Survey of Simultaneous Localizationand Mapping SLAM.pdf</t>
+    <t>A Survey of Simultaneous Localizationand Mapping SLAM</t>
   </si>
   <si>
     <t>Baichuan Huang等</t>
@@ -77,6 +77,36 @@
   </si>
   <si>
     <t>梳理了很多技术名词</t>
+  </si>
+  <si>
+    <t>Survey-coverage-path-planning for Robotics</t>
+  </si>
+  <si>
+    <t>E Galceran, M Carreras</t>
+  </si>
+  <si>
+    <t>Robotics and Autonomous systems</t>
+  </si>
+  <si>
+    <t>1. 机器人必须完全穿过覆盖它的目标区域中的所有点。2. 机器人必须填充该区域而没有重叠的路径。3. 需要连续和顺序的操作，而无需重复任何路径。4. 机器人必须避开所有的障碍。5. 应使用简单的运动轨迹（例如，直线或圆）（便于控制）。6. 在可用条件下，需要一条“最佳”路径</t>
+  </si>
+  <si>
+    <t>全覆盖路径问题的高引综述</t>
+  </si>
+  <si>
+    <t>Semantics for Robotic Mapping Perception and Interaction A Survey</t>
+  </si>
+  <si>
+    <t>Sourav Garg1∗
+, Niko S¨underhauf1
+, Feras Dayoub1
+, Douglas Morrison1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foundations and Trends® in Robotics</t>
+  </si>
+  <si>
+    <t>目前移动机器人仅在一些小众领域应用，因为不“understand”世界，所以很难部署到复杂的有人的环境。这种“理解”就需要语义与机器人技术相遇。本文旨在提供整个机器人领域语义的开发和使用的统一概述。将与机器人有关的语义论文分为四类。四类语义研究由技术、知识和训练相关的增强器补充，并产生一系列机器人应用。主要涉及提取语义、使用语义或两者的组合。</t>
   </si>
 </sst>
 </file>
@@ -84,10 +114,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -122,7 +152,81 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,78 +248,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,29 +273,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,187 +296,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,22 +493,22 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -499,17 +529,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,16 +557,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,6 +572,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -565,10 +595,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -577,133 +607,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1068,13 +1098,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="3" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="62.3333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5555555555556" style="1" customWidth="1"/>
@@ -1163,11 +1193,50 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" ht="62.4" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" ht="93.6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age" tooltip="Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age"/>
     <hyperlink ref="A3" r:id="rId2" display="无人系统视觉SLAM技术发展现状简析"/>
-    <hyperlink ref="A4" r:id="rId3" display="A Survey of Simultaneous Localizationand Mapping SLAM.pdf"/>
+    <hyperlink ref="A4" r:id="rId3" display="A Survey of Simultaneous Localizationand Mapping SLAM"/>
+    <hyperlink ref="A5" r:id="rId4" display="Survey-coverage-path-planning for Robotics"/>
+    <hyperlink ref="A6" r:id="rId5" display="Semantics for Robotic Mapping Perception and Interaction A Survey"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
update my slam note
</commit_message>
<xml_diff>
--- a/Robotics_and_Slam/2_slam_paper.xlsx
+++ b/Robotics_and_Slam/2_slam_paper.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>title</t>
   </si>
@@ -107,6 +107,19 @@
   </si>
   <si>
     <t>目前移动机器人仅在一些小众领域应用，因为不“understand”世界，所以很难部署到复杂的有人的环境。这种“理解”就需要语义与机器人技术相遇。本文旨在提供整个机器人领域语义的开发和使用的统一概述。将与机器人有关的语义论文分为四类。四类语义研究由技术、知识和训练相关的增强器补充，并产生一系列机器人应用。主要涉及提取语义、使用语义或两者的组合。</t>
+  </si>
+  <si>
+    <t>6_室内移动机器人的SLAM算法综述.caj</t>
+  </si>
+  <si>
+    <t>田野</t>
+  </si>
+  <si>
+    <t>计算机科学</t>
+  </si>
+  <si>
+    <t>介绍了SLAM 算法框架、分类以及经典室
+内 SLAM 算法的论述</t>
   </si>
 </sst>
 </file>
@@ -114,10 +127,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -152,6 +165,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -159,23 +179,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -194,44 +230,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -248,21 +246,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -271,6 +254,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -281,7 +271,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,187 +309,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,30 +500,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -525,15 +514,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,11 +544,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,6 +574,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -595,10 +608,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -607,19 +620,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -628,112 +641,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1098,13 +1111,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="62.3333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5555555555556" style="1" customWidth="1"/>
@@ -1228,6 +1241,23 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="31.2" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>